<commit_message>
Sumsung scraping code added
</commit_message>
<xml_diff>
--- a/Scrape_Bot1/Data/MasterULRs.xlsx
+++ b/Scrape_Bot1/Data/MasterULRs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\RPA_WebScraping\Scrape_Bot1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D4F4F1-8D77-4C59-BA31-A4FF6122ADB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E57BFB-434A-4CA0-9C74-9C274452A1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Category</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>Ovens</t>
+  </si>
+  <si>
+    <t>https://www.samsung.com/in/microwave-ovens/all-microwave-ovens/</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Samsung</t>
   </si>
 </sst>
 </file>
@@ -393,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,7 +413,7 @@
     <col min="1" max="1" width="9.109375" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -461,6 +470,20 @@
       </c>
       <c r="D4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>